<commit_message>
added all data route
</commit_message>
<xml_diff>
--- a/flask_backend/models/City_excell.xlsx
+++ b/flask_backend/models/City_excell.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedron\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\VacancyApp\flask_backend\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDE95A7-0426-44BB-AEBB-C837A33D35FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F4972-8440-4777-9B2F-3F47C8A4A73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -2196,17 +2196,10 @@
     <t>place</t>
   </si>
   <si>
-    <t>15.588398  73.947827</t>
-  </si>
-  <si>
     <t xml:space="preserve">  15.587195 73.947497</t>
   </si>
   <si>
     <t xml:space="preserve">  15.586768 73.948034</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 
-15.587436 73.947343</t>
   </si>
   <si>
     <t xml:space="preserve">  15.587300 73.947480</t>
@@ -2503,6 +2496,12 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15.587436 73.947343</t>
+  </si>
+  <si>
+    <t>15.588398 73.947827</t>
   </si>
 </sst>
 </file>
@@ -3041,7 +3040,7 @@
   <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3062,16 +3061,16 @@
         <v>234</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="4" t="s">
         <v>327</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>328</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3082,7 +3081,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>235</v>
+        <v>329</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
@@ -3091,7 +3090,7 @@
         <v>120</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3102,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -3120,7 +3119,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
@@ -3138,7 +3137,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>238</v>
+        <v>328</v>
       </c>
       <c r="D5" s="6">
         <v>30</v>
@@ -3147,7 +3146,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3158,7 +3157,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D6" s="6">
         <v>10</v>
@@ -3176,7 +3175,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D7" s="6">
         <v>30</v>
@@ -3194,7 +3193,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D8" s="6">
         <v>15</v>
@@ -3212,7 +3211,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D9" s="6">
         <v>20</v>
@@ -3230,7 +3229,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D10" s="6">
         <v>5</v>
@@ -3248,7 +3247,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D11" s="6">
         <v>10</v>
@@ -3266,7 +3265,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D12" s="6">
         <v>20</v>
@@ -3275,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3286,7 +3285,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D13" s="6">
         <v>0</v>
@@ -3295,7 +3294,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3306,7 +3305,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D14" s="6">
         <v>0</v>
@@ -3315,7 +3314,7 @@
         <v>180</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3326,7 +3325,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D15" s="6">
         <v>12</v>
@@ -3335,7 +3334,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3346,7 +3345,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D16" s="6">
         <v>10</v>
@@ -3355,7 +3354,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="41.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -3366,7 +3365,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D17" s="6">
         <v>0</v>
@@ -3375,7 +3374,7 @@
         <v>80</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="41.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -3386,7 +3385,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D18" s="6">
         <v>7</v>
@@ -3395,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="41.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -3406,7 +3405,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D19" s="6">
         <v>0</v>
@@ -3415,7 +3414,7 @@
         <v>70</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3426,7 +3425,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D20" s="6">
         <v>0</v>
@@ -3444,7 +3443,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D21" s="6">
         <v>0</v>
@@ -3462,7 +3461,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D22" s="6">
         <v>10</v>
@@ -3480,7 +3479,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D23" s="6">
         <v>0</v>
@@ -3498,7 +3497,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D24" s="6">
         <v>10</v>
@@ -3516,7 +3515,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D25" s="15">
         <v>25</v>
@@ -3548,7 +3547,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D27" s="6">
         <v>20</v>
@@ -3566,7 +3565,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D28" s="6">
         <v>10</v>
@@ -3584,7 +3583,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D29" s="6">
         <v>5</v>
@@ -3602,7 +3601,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D30" s="6">
         <v>5</v>
@@ -3620,7 +3619,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D31" s="6">
         <v>50</v>
@@ -3629,7 +3628,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
@@ -3637,10 +3636,10 @@
         <v>141</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D32" s="18">
         <v>30</v>
@@ -3657,10 +3656,10 @@
         <v>141</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D33" s="18">
         <v>30</v>
@@ -3677,10 +3676,10 @@
         <v>141</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D34" s="18">
         <v>30</v>
@@ -3697,10 +3696,10 @@
         <v>141</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D35" s="18">
         <v>30</v>
@@ -3717,10 +3716,10 @@
         <v>141</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D36" s="18">
         <v>30</v>
@@ -3737,10 +3736,10 @@
         <v>141</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D37" s="18">
         <v>30</v>
@@ -3757,10 +3756,10 @@
         <v>141</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D38" s="18">
         <v>30</v>
@@ -3777,10 +3776,10 @@
         <v>141</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D39" s="18">
         <v>30</v>
@@ -3797,10 +3796,10 @@
         <v>141</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D40" s="18">
         <v>30</v>
@@ -3817,10 +3816,10 @@
         <v>141</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D41" s="18">
         <v>30</v>
@@ -3840,7 +3839,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D42" s="10">
         <v>320</v>
@@ -3860,7 +3859,7 @@
         <v>33</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D43" s="10">
         <v>500</v>
@@ -3880,7 +3879,7 @@
         <v>34</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D44" s="10">
         <v>0</v>
@@ -3900,7 +3899,7 @@
         <v>36</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D45" s="10">
         <v>100</v>
@@ -3924,10 +3923,10 @@
         <v>143</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D47" s="6">
         <v>40</v>
@@ -3944,10 +3943,10 @@
         <v>143</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D48" s="6">
         <v>40</v>
@@ -3956,7 +3955,7 @@
         <v>70</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -3964,10 +3963,10 @@
         <v>143</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D49" s="6">
         <v>25</v>
@@ -3976,7 +3975,7 @@
         <v>50</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -3984,10 +3983,10 @@
         <v>143</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D50" s="6">
         <v>25</v>
@@ -3996,7 +3995,7 @@
         <v>50</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -4004,10 +4003,10 @@
         <v>143</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D51" s="6">
         <v>60</v>
@@ -4016,7 +4015,7 @@
         <v>70</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
@@ -4027,7 +4026,7 @@
         <v>38</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D52" s="6">
         <v>300</v>
@@ -4036,7 +4035,7 @@
         <v>400</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
@@ -4047,7 +4046,7 @@
         <v>39</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D53" s="6">
         <v>100</v>
@@ -4056,7 +4055,7 @@
         <v>200</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -4064,10 +4063,10 @@
         <v>143</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D54" s="6">
         <v>15</v>
@@ -4076,7 +4075,7 @@
         <v>50</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
@@ -4127,7 +4126,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D57" s="3">
         <v>450</v>
@@ -4147,7 +4146,7 @@
         <v>44</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D58" s="3">
         <v>50</v>
@@ -4167,7 +4166,7 @@
         <v>45</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D59" s="3">
         <v>61</v>
@@ -4187,7 +4186,7 @@
         <v>45</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D60" s="3">
         <v>25</v>
@@ -4207,7 +4206,7 @@
         <v>46</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D61" s="3">
         <v>80</v>
@@ -4227,7 +4226,7 @@
         <v>47</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D62" s="3">
         <v>30</v>
@@ -4247,7 +4246,7 @@
         <v>48</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D63" s="3">
         <v>150</v>
@@ -4267,7 +4266,7 @@
         <v>49</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D64" s="3">
         <v>200</v>
@@ -4287,7 +4286,7 @@
         <v>50</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D65" s="3">
         <v>150</v>
@@ -4307,7 +4306,7 @@
         <v>51</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D66" s="3">
         <v>276</v>
@@ -4327,7 +4326,7 @@
         <v>52</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D67" s="3">
         <v>249</v>
@@ -4347,7 +4346,7 @@
         <v>53</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D68" s="3">
         <v>198</v>
@@ -4367,7 +4366,7 @@
         <v>54</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D69" s="3">
         <v>65</v>
@@ -4387,7 +4386,7 @@
         <v>55</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D70" s="3">
         <v>60</v>
@@ -4407,7 +4406,7 @@
         <v>56</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D71" s="3">
         <v>60</v>
@@ -4427,7 +4426,7 @@
         <v>57</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D72" s="3">
         <v>97</v>
@@ -4447,7 +4446,7 @@
         <v>58</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D73" s="3">
         <v>1200</v>
@@ -4631,7 +4630,7 @@
         <v>147</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>160</v>
@@ -5496,7 +5495,7 @@
         <v>151</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C130" s="10" t="s">
         <v>196</v>
@@ -5516,7 +5515,7 @@
         <v>151</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C131" s="10" t="s">
         <v>196</v>
@@ -5596,7 +5595,7 @@
         <v>151</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C135" s="10" t="s">
         <v>200</v>
@@ -5956,7 +5955,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C153" s="10" t="s">
         <v>214</v>
@@ -6156,7 +6155,7 @@
         <v>151</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C163" s="10" t="s">
         <v>224</v>

</xml_diff>